<commit_message>
changes has been updated
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -25,55 +25,55 @@
     <x:t>10</x:t>
   </x:si>
   <x:si>
-    <x:t>724.65</x:t>
+    <x:t>732.91</x:t>
   </x:si>
   <x:si>
     <x:t>50</x:t>
   </x:si>
   <x:si>
-    <x:t>3623.25</x:t>
+    <x:t>3664.53</x:t>
   </x:si>
   <x:si>
     <x:t>90</x:t>
   </x:si>
   <x:si>
-    <x:t>6521.85</x:t>
+    <x:t>6596.15</x:t>
   </x:si>
   <x:si>
     <x:t>110</x:t>
   </x:si>
   <x:si>
-    <x:t>7971.15</x:t>
+    <x:t>8061.96</x:t>
   </x:si>
   <x:si>
     <x:t>210</x:t>
   </x:si>
   <x:si>
-    <x:t>15217.65</x:t>
+    <x:t>15391.01</x:t>
   </x:si>
   <x:si>
     <x:t>39</x:t>
   </x:si>
   <x:si>
-    <x:t>2826.14</x:t>
+    <x:t>2858.33</x:t>
   </x:si>
   <x:si>
     <x:t>48</x:t>
   </x:si>
   <x:si>
-    <x:t>3478.32</x:t>
+    <x:t>3517.94</x:t>
   </x:si>
   <x:si>
     <x:t>66</x:t>
   </x:si>
   <x:si>
-    <x:t>4782.69</x:t>
+    <x:t>4837.17</x:t>
   </x:si>
   <x:si>
     <x:t>32</x:t>
   </x:si>
   <x:si>
-    <x:t>2318.88</x:t>
+    <x:t>2345.30</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>